<commit_message>
aligned Release configuration. Also removed _CRT_SECURE_NO_WARNINGS from sTimer
</commit_message>
<xml_diff>
--- a/TestSets.xlsx
+++ b/TestSets.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="54">
   <si>
     <t>SCGD</t>
   </si>
@@ -185,6 +185,9 @@
   <si>
     <t>050</t>
   </si>
+  <si>
+    <t>MEM!</t>
+  </si>
 </sst>
 </file>
 
@@ -207,12 +210,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -236,7 +245,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -261,6 +270,7 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -640,7 +650,7 @@
       <pane xSplit="1" ySplit="4" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
+      <selection pane="bottomRight" activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2890,6 +2900,9 @@
       </c>
     </row>
     <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A31" s="12" t="s">
+        <v>53</v>
+      </c>
       <c r="B31" t="s">
         <v>3</v>
       </c>
@@ -2924,50 +2937,53 @@
       </c>
       <c r="K31" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i0.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i0.xml Config.NoInclude/Engines/STD-2-2-1.xml MEM!</v>
       </c>
       <c r="L31" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i1.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i1.xml Config.NoInclude/Engines/STD-2-2-1.xml MEM!</v>
       </c>
       <c r="M31" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i2.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i2.xml Config.NoInclude/Engines/STD-2-2-1.xml MEM!</v>
       </c>
       <c r="N31" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i3.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i3.xml Config.NoInclude/Engines/STD-2-2-1.xml MEM!</v>
       </c>
       <c r="O31" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i4.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i4.xml Config.NoInclude/Engines/STD-2-2-1.xml MEM!</v>
       </c>
       <c r="P31" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i5.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i5.xml Config.NoInclude/Engines/STD-2-2-1.xml MEM!</v>
       </c>
       <c r="Q31" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i0b.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i0b.xml Config.NoInclude/Engines/STD-2-2-1.xml MEM!</v>
       </c>
       <c r="R31" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i1b.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i1b.xml Config.NoInclude/Engines/STD-2-2-1.xml MEM!</v>
       </c>
       <c r="S31" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i2b.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i2b.xml Config.NoInclude/Engines/STD-2-2-1.xml MEM!</v>
       </c>
       <c r="T31" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i3b.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i3b.xml Config.NoInclude/Engines/STD-2-2-1.xml MEM!</v>
       </c>
       <c r="U31" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i4b.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i4b.xml Config.NoInclude/Engines/STD-2-2-1.xml MEM!</v>
       </c>
     </row>
     <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>7252</v>
+      </c>
       <c r="B32" t="s">
         <v>3</v>
       </c>
@@ -3002,50 +3018,53 @@
       </c>
       <c r="K32" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0.xml Config.NoInclude/Engines/STD-2-2-1.xml 7252</v>
       </c>
       <c r="L32" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i1.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i1.xml Config.NoInclude/Engines/STD-2-2-1.xml 7252</v>
       </c>
       <c r="M32" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i2.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i2.xml Config.NoInclude/Engines/STD-2-2-1.xml 7252</v>
       </c>
       <c r="N32" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i3.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i3.xml Config.NoInclude/Engines/STD-2-2-1.xml 7252</v>
       </c>
       <c r="O32" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i4.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i4.xml Config.NoInclude/Engines/STD-2-2-1.xml 7252</v>
       </c>
       <c r="P32" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i5.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i5.xml Config.NoInclude/Engines/STD-2-2-1.xml 7252</v>
       </c>
       <c r="Q32" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0b.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0b.xml Config.NoInclude/Engines/STD-2-2-1.xml 7252</v>
       </c>
       <c r="R32" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i1b.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i1b.xml Config.NoInclude/Engines/STD-2-2-1.xml 7252</v>
       </c>
       <c r="S32" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i2b.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i2b.xml Config.NoInclude/Engines/STD-2-2-1.xml 7252</v>
       </c>
       <c r="T32" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i3b.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i3b.xml Config.NoInclude/Engines/STD-2-2-1.xml 7252</v>
       </c>
       <c r="U32" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i4b.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
-      </c>
-    </row>
-    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i4b.xml Config.NoInclude/Engines/STD-2-2-1.xml 7252</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>4880</v>
+      </c>
       <c r="B33" t="s">
         <v>3</v>
       </c>
@@ -3080,50 +3099,53 @@
       </c>
       <c r="K33" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i0.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i0.xml Config.NoInclude/Engines/STD-2-2-1.xml 4880</v>
       </c>
       <c r="L33" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i1.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i1.xml Config.NoInclude/Engines/STD-2-2-1.xml 4880</v>
       </c>
       <c r="M33" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i2.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i2.xml Config.NoInclude/Engines/STD-2-2-1.xml 4880</v>
       </c>
       <c r="N33" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i3.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i3.xml Config.NoInclude/Engines/STD-2-2-1.xml 4880</v>
       </c>
       <c r="O33" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i4.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i4.xml Config.NoInclude/Engines/STD-2-2-1.xml 4880</v>
       </c>
       <c r="P33" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i5.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i5.xml Config.NoInclude/Engines/STD-2-2-1.xml 4880</v>
       </c>
       <c r="Q33" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i0b.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i0b.xml Config.NoInclude/Engines/STD-2-2-1.xml 4880</v>
       </c>
       <c r="R33" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i1b.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i1b.xml Config.NoInclude/Engines/STD-2-2-1.xml 4880</v>
       </c>
       <c r="S33" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i2b.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i2b.xml Config.NoInclude/Engines/STD-2-2-1.xml 4880</v>
       </c>
       <c r="T33" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i3b.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i3b.xml Config.NoInclude/Engines/STD-2-2-1.xml 4880</v>
       </c>
       <c r="U33" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i4b.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
-      </c>
-    </row>
-    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i4b.xml Config.NoInclude/Engines/STD-2-2-1.xml 4880</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A34" s="12" t="s">
+        <v>53</v>
+      </c>
       <c r="B34" t="s">
         <v>3</v>
       </c>
@@ -3158,50 +3180,53 @@
       </c>
       <c r="K34" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i0.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i0.xml Config.NoInclude/Engines/STD-2-2-1.xml MEM!</v>
       </c>
       <c r="L34" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i1.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i1.xml Config.NoInclude/Engines/STD-2-2-1.xml MEM!</v>
       </c>
       <c r="M34" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i2.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i2.xml Config.NoInclude/Engines/STD-2-2-1.xml MEM!</v>
       </c>
       <c r="N34" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i3.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i3.xml Config.NoInclude/Engines/STD-2-2-1.xml MEM!</v>
       </c>
       <c r="O34" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i4.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i4.xml Config.NoInclude/Engines/STD-2-2-1.xml MEM!</v>
       </c>
       <c r="P34" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i5.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i5.xml Config.NoInclude/Engines/STD-2-2-1.xml MEM!</v>
       </c>
       <c r="Q34" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i0b.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i0b.xml Config.NoInclude/Engines/STD-2-2-1.xml MEM!</v>
       </c>
       <c r="R34" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i1b.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i1b.xml Config.NoInclude/Engines/STD-2-2-1.xml MEM!</v>
       </c>
       <c r="S34" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i2b.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i2b.xml Config.NoInclude/Engines/STD-2-2-1.xml MEM!</v>
       </c>
       <c r="T34" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i3b.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i3b.xml Config.NoInclude/Engines/STD-2-2-1.xml MEM!</v>
       </c>
       <c r="U34" t="str">
         <f t="shared" si="7"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i4b.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
-      </c>
-    </row>
-    <row r="35" spans="2:21" x14ac:dyDescent="0.25">
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i4b.xml Config.NoInclude/Engines/STD-2-2-1.xml MEM!</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>3476</v>
+      </c>
       <c r="B35" t="s">
         <v>3</v>
       </c>
@@ -3236,50 +3261,50 @@
       </c>
       <c r="K35" t="str">
         <f t="shared" ref="K35:U44" si="8">"zzz Infer "&amp;$A$2&amp;" Config.NoInclude/Client.xml "&amp;$G35&amp;" "&amp;K$2&amp;" "&amp;$H35&amp;" "&amp;$A35</f>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0.xml Config.NoInclude/Engines/STD-2-2-1.xml 3476</v>
       </c>
       <c r="L35" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i1.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i1.xml Config.NoInclude/Engines/STD-2-2-1.xml 3476</v>
       </c>
       <c r="M35" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i2.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i2.xml Config.NoInclude/Engines/STD-2-2-1.xml 3476</v>
       </c>
       <c r="N35" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i3.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i3.xml Config.NoInclude/Engines/STD-2-2-1.xml 3476</v>
       </c>
       <c r="O35" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i4.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i4.xml Config.NoInclude/Engines/STD-2-2-1.xml 3476</v>
       </c>
       <c r="P35" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i5.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i5.xml Config.NoInclude/Engines/STD-2-2-1.xml 3476</v>
       </c>
       <c r="Q35" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0b.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0b.xml Config.NoInclude/Engines/STD-2-2-1.xml 3476</v>
       </c>
       <c r="R35" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i1b.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i1b.xml Config.NoInclude/Engines/STD-2-2-1.xml 3476</v>
       </c>
       <c r="S35" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i2b.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i2b.xml Config.NoInclude/Engines/STD-2-2-1.xml 3476</v>
       </c>
       <c r="T35" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i3b.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i3b.xml Config.NoInclude/Engines/STD-2-2-1.xml 3476</v>
       </c>
       <c r="U35" t="str">
         <f t="shared" si="8"/>
-        <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i4b.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
-      </c>
-    </row>
-    <row r="36" spans="2:21" x14ac:dyDescent="0.25">
+        <v>zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i4b.xml Config.NoInclude/Engines/STD-2-2-1.xml 3476</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>3</v>
       </c>
@@ -3357,7 +3382,7 @@
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i4b.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
       </c>
     </row>
-    <row r="37" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>3</v>
       </c>
@@ -3435,7 +3460,7 @@
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i4b.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
       </c>
     </row>
-    <row r="38" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>3</v>
       </c>
@@ -3513,7 +3538,7 @@
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i4b.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
       </c>
     </row>
-    <row r="39" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>3</v>
       </c>
@@ -3591,7 +3616,7 @@
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i4b.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
       </c>
     </row>
-    <row r="40" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>3</v>
       </c>
@@ -3669,7 +3694,7 @@
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i4b.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
       </c>
     </row>
-    <row r="41" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>0</v>
       </c>
@@ -3747,7 +3772,7 @@
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i4b.xml Config.NoInclude/Engines/SCGD-2.xml </v>
       </c>
     </row>
-    <row r="42" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>0</v>
       </c>
@@ -3825,7 +3850,7 @@
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i4b.xml Config.NoInclude/Engines/SCGD-2.xml </v>
       </c>
     </row>
-    <row r="43" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>0</v>
       </c>
@@ -3903,7 +3928,7 @@
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i4b.xml Config.NoInclude/Engines/SCGD-2.xml </v>
       </c>
     </row>
-    <row r="44" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>0</v>
       </c>
@@ -3981,7 +4006,7 @@
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i4b.xml Config.NoInclude/Engines/SCGD-2.xml </v>
       </c>
     </row>
-    <row r="45" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>0</v>
       </c>
@@ -4059,7 +4084,7 @@
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i4b.xml Config.NoInclude/Engines/SCGD-2.xml </v>
       </c>
     </row>
-    <row r="46" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>0</v>
       </c>
@@ -4137,7 +4162,7 @@
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i4b.xml Config.NoInclude/Engines/SCGD-2.xml </v>
       </c>
     </row>
-    <row r="47" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>0</v>
       </c>
@@ -4215,7 +4240,7 @@
         <v xml:space="preserve">zzz Infer 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i4b.xml Config.NoInclude/Engines/SCGD-2.xml </v>
       </c>
     </row>
-    <row r="48" spans="2:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>0</v>
       </c>
@@ -5883,7 +5908,7 @@
         <v>Config.NoInclude/DataSets/12000.xml</v>
       </c>
       <c r="J69" t="str">
-        <f t="shared" ref="J69:J100" si="19">"zzz Both "&amp;$A$2&amp;" Config.NoInclude/Client.xml "&amp;G69&amp;" "&amp;I69&amp;" "&amp;H69</f>
+        <f t="shared" ref="J69:J76" si="19">"zzz Both "&amp;$A$2&amp;" Config.NoInclude/Client.xml "&amp;G69&amp;" "&amp;I69&amp;" "&amp;H69</f>
         <v>zzz Both 21 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/SCGD-2-2-1.xml</v>
       </c>
       <c r="K69" t="str">

</xml_diff>

<commit_message>
added new infer sets with BatchSamplesCnt=1
</commit_message>
<xml_diff>
--- a/TestSets.xlsx
+++ b/TestSets.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21420" windowHeight="6456" activeTab="1"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="21420" windowHeight="6456" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="21-Desc" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="54">
   <si>
     <t>SCGD</t>
   </si>
@@ -181,6 +181,15 @@
   </si>
   <si>
     <t>Infer0d cmd</t>
+  </si>
+  <si>
+    <t>Config.NoInclude/DataSets/i0a-bsc1.xml</t>
+  </si>
+  <si>
+    <t>Config.NoInclude/DataSets/i0b-bsc1.xml</t>
+  </si>
+  <si>
+    <t>Config.NoInclude/DataSets/i0c-bsc1.xml</t>
   </si>
 </sst>
 </file>
@@ -639,13 +648,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:Q76"/>
+  <dimension ref="A1:T76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="4" topLeftCell="M41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="4" topLeftCell="Q41" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="A77" sqref="A77"/>
+      <selection pane="bottomRight" activeCell="R41" sqref="R41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -661,9 +670,11 @@
     <col min="9" max="9" width="35.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.5546875" customWidth="1"/>
     <col min="11" max="17" width="32" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="34.77734375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="34.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>11</v>
       </c>
@@ -672,7 +683,7 @@
       </c>
       <c r="N1" s="2"/>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>22</v>
       </c>
@@ -697,8 +708,17 @@
       <c r="Q2" s="4" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="K3" s="4"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
@@ -707,7 +727,7 @@
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
     </row>
-    <row r="4" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
@@ -760,7 +780,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>6556</v>
       </c>
@@ -825,7 +845,7 @@
         <v>zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/STD-2.xml 6556</v>
       </c>
     </row>
-    <row r="6" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>9048</v>
       </c>
@@ -890,7 +910,7 @@
         <v>zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/STD-2.xml 9048</v>
       </c>
     </row>
-    <row r="7" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>5368</v>
       </c>
@@ -955,7 +975,7 @@
         <v>zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/STD-2.xml 5368</v>
       </c>
     </row>
-    <row r="8" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>1624</v>
       </c>
@@ -1020,7 +1040,7 @@
         <v>zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/STD-2.xml 1624</v>
       </c>
     </row>
-    <row r="9" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>9368</v>
       </c>
@@ -1085,7 +1105,7 @@
         <v>zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/STD-2.xml 9368</v>
       </c>
     </row>
-    <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>3400</v>
       </c>
@@ -1150,7 +1170,7 @@
         <v>zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/STD-2.xml 3400</v>
       </c>
     </row>
-    <row r="11" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>9372</v>
       </c>
@@ -1215,7 +1235,7 @@
         <v>zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/STD-2.xml 9372</v>
       </c>
     </row>
-    <row r="12" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>3576</v>
       </c>
@@ -1280,7 +1300,7 @@
         <v>zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/STD-2.xml 3576</v>
       </c>
     </row>
-    <row r="13" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>1980</v>
       </c>
@@ -1345,7 +1365,7 @@
         <v>zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/STD-2.xml 1980</v>
       </c>
     </row>
-    <row r="14" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>8052</v>
       </c>
@@ -1410,7 +1430,7 @@
         <v>zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/STD-2.xml 8052</v>
       </c>
     </row>
-    <row r="15" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>5532</v>
       </c>
@@ -1475,7 +1495,7 @@
         <v>zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/STD-2.xml 5532</v>
       </c>
     </row>
-    <row r="16" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>6348</v>
       </c>
@@ -1540,7 +1560,7 @@
         <v>zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/STD-2.xml 6348</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>9488</v>
       </c>
@@ -2320,7 +2340,7 @@
         <v>zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/STD-1-1.xml 5656</v>
       </c>
     </row>
-    <row r="29" spans="1:17" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" s="8" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29" s="8">
         <v>2416</v>
       </c>
@@ -2580,7 +2600,7 @@
         <v>zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/STD-2-2-1.xml 7252</v>
       </c>
     </row>
-    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>4880</v>
       </c>
@@ -2645,7 +2665,7 @@
         <v>zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/STD-2-2-1.xml 4880</v>
       </c>
     </row>
-    <row r="34" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="12" t="s">
         <v>43</v>
       </c>
@@ -2710,7 +2730,7 @@
         <v>zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/STD-2-2-1.xml MEM!</v>
       </c>
     </row>
-    <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>3476</v>
       </c>
@@ -2747,7 +2767,7 @@
         <v>zzz Both 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/18000.xml Config.NoInclude/Engines/STD-2-2-1.xml</v>
       </c>
       <c r="K35" t="str">
-        <f t="shared" ref="K35:Q44" si="8">"zzz Infer "&amp;$A$2&amp;" Config.NoInclude/Client.xml "&amp;$G35&amp;" "&amp;K$2&amp;" "&amp;$H35&amp;" "&amp;$A35</f>
+        <f t="shared" ref="K35:T44" si="8">"zzz Infer "&amp;$A$2&amp;" Config.NoInclude/Client.xml "&amp;$G35&amp;" "&amp;K$2&amp;" "&amp;$H35&amp;" "&amp;$A35</f>
         <v>zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0.xml Config.NoInclude/Engines/STD-2-2-1.xml 3476</v>
       </c>
       <c r="L35" t="str">
@@ -2775,7 +2795,7 @@
         <v>zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/STD-2-2-1.xml 3476</v>
       </c>
     </row>
-    <row r="36" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>3</v>
       </c>
@@ -2837,7 +2857,7 @@
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
       </c>
     </row>
-    <row r="37" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B37" t="s">
         <v>3</v>
       </c>
@@ -2899,7 +2919,7 @@
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
       </c>
     </row>
-    <row r="38" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
         <v>3</v>
       </c>
@@ -2961,7 +2981,7 @@
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
       </c>
     </row>
-    <row r="39" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>3</v>
       </c>
@@ -3023,7 +3043,7 @@
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
       </c>
     </row>
-    <row r="40" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>3</v>
       </c>
@@ -3085,7 +3105,7 @@
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/STD-2-2-1.xml </v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41" s="11">
         <v>9860</v>
       </c>
@@ -3149,8 +3169,20 @@
         <f t="shared" si="8"/>
         <v>zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/SCGD-2.xml 9860</v>
       </c>
-    </row>
-    <row r="42" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+      <c r="R41" t="str">
+        <f t="shared" si="8"/>
+        <v>zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0a-bsc1.xml Config.NoInclude/Engines/SCGD-2.xml 9860</v>
+      </c>
+      <c r="S41" t="str">
+        <f t="shared" si="8"/>
+        <v>zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0b-bsc1.xml Config.NoInclude/Engines/SCGD-2.xml 9860</v>
+      </c>
+      <c r="T41" t="str">
+        <f t="shared" si="8"/>
+        <v>zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0c-bsc1.xml Config.NoInclude/Engines/SCGD-2.xml 9860</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
         <v>0</v>
       </c>
@@ -3212,7 +3244,7 @@
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/SCGD-2.xml </v>
       </c>
     </row>
-    <row r="43" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
         <v>0</v>
       </c>
@@ -3274,7 +3306,7 @@
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/SCGD-2.xml </v>
       </c>
     </row>
-    <row r="44" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>0</v>
       </c>
@@ -3336,7 +3368,7 @@
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/SCGD-2.xml </v>
       </c>
     </row>
-    <row r="45" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>0</v>
       </c>
@@ -3370,7 +3402,7 @@
         <v>zzz Both 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/12000.xml Config.NoInclude/Engines/SCGD-2.xml</v>
       </c>
       <c r="K45" t="str">
-        <f t="shared" ref="K45:Q54" si="13">"zzz Infer "&amp;$A$2&amp;" Config.NoInclude/Client.xml "&amp;$G45&amp;" "&amp;K$2&amp;" "&amp;$H45&amp;" "&amp;$A45</f>
+        <f t="shared" ref="K45:T54" si="13">"zzz Infer "&amp;$A$2&amp;" Config.NoInclude/Client.xml "&amp;$G45&amp;" "&amp;K$2&amp;" "&amp;$H45&amp;" "&amp;$A45</f>
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i0.xml Config.NoInclude/Engines/SCGD-2.xml </v>
       </c>
       <c r="L45" t="str">
@@ -3398,7 +3430,7 @@
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/SCGD-2.xml </v>
       </c>
     </row>
-    <row r="46" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
         <v>0</v>
       </c>
@@ -3460,7 +3492,7 @@
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/SCGD-2.xml </v>
       </c>
     </row>
-    <row r="47" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
         <v>0</v>
       </c>
@@ -3522,7 +3554,7 @@
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/SCGD-2.xml </v>
       </c>
     </row>
-    <row r="48" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
         <v>0</v>
       </c>
@@ -3584,7 +3616,7 @@
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/SCGD-2.xml </v>
       </c>
     </row>
-    <row r="49" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
         <v>0</v>
       </c>
@@ -3646,7 +3678,7 @@
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/SCGD-2.xml </v>
       </c>
     </row>
-    <row r="50" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>0</v>
       </c>
@@ -3708,7 +3740,7 @@
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/SCGD-2.xml </v>
       </c>
     </row>
-    <row r="51" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>0</v>
       </c>
@@ -3770,7 +3802,7 @@
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/SCGD-2.xml </v>
       </c>
     </row>
-    <row r="52" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>0</v>
       </c>
@@ -3832,7 +3864,7 @@
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/SCGD-2.xml </v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A53" s="11">
         <v>3508</v>
       </c>
@@ -3896,8 +3928,20 @@
         <f t="shared" si="13"/>
         <v>zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/SCGD-1-1.xml 3508</v>
       </c>
-    </row>
-    <row r="54" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+      <c r="R53" t="str">
+        <f t="shared" si="13"/>
+        <v>zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0a-bsc1.xml Config.NoInclude/Engines/SCGD-1-1.xml 3508</v>
+      </c>
+      <c r="S53" t="str">
+        <f t="shared" si="13"/>
+        <v>zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0b-bsc1.xml Config.NoInclude/Engines/SCGD-1-1.xml 3508</v>
+      </c>
+      <c r="T53" t="str">
+        <f t="shared" si="13"/>
+        <v>zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0c-bsc1.xml Config.NoInclude/Engines/SCGD-1-1.xml 3508</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
         <v>0</v>
       </c>
@@ -3959,7 +4003,7 @@
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/SCGD-1-1.xml </v>
       </c>
     </row>
-    <row r="55" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>0</v>
       </c>
@@ -4021,7 +4065,7 @@
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/SCGD-1-1.xml </v>
       </c>
     </row>
-    <row r="56" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>0</v>
       </c>
@@ -4083,7 +4127,7 @@
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/SCGD-1-1.xml </v>
       </c>
     </row>
-    <row r="57" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>0</v>
       </c>
@@ -4145,7 +4189,7 @@
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/SCGD-1-1.xml </v>
       </c>
     </row>
-    <row r="58" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
         <v>0</v>
       </c>
@@ -4207,7 +4251,7 @@
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/SCGD-1-1.xml </v>
       </c>
     </row>
-    <row r="59" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
         <v>0</v>
       </c>
@@ -4269,7 +4313,7 @@
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/SCGD-1-1.xml </v>
       </c>
     </row>
-    <row r="60" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B60" t="s">
         <v>0</v>
       </c>
@@ -4331,7 +4375,7 @@
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/SCGD-1-1.xml </v>
       </c>
     </row>
-    <row r="61" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>0</v>
       </c>
@@ -4393,7 +4437,7 @@
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/SCGD-1-1.xml </v>
       </c>
     </row>
-    <row r="62" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B62" t="s">
         <v>0</v>
       </c>
@@ -4455,7 +4499,7 @@
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/SCGD-1-1.xml </v>
       </c>
     </row>
-    <row r="63" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>0</v>
       </c>
@@ -4517,7 +4561,7 @@
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/SCGD-1-1.xml </v>
       </c>
     </row>
-    <row r="64" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B64" t="s">
         <v>0</v>
       </c>
@@ -4579,7 +4623,7 @@
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/SCGD-1-1.xml </v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A65" s="11">
         <v>4916</v>
       </c>
@@ -4616,7 +4660,7 @@
         <v>zzz Both 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/06000.xml Config.NoInclude/Engines/SCGD-2-2-1.xml</v>
       </c>
       <c r="K65" t="str">
-        <f t="shared" ref="K65:Q76" si="15">"zzz Infer "&amp;$A$2&amp;" Config.NoInclude/Client.xml "&amp;$G65&amp;" "&amp;K$2&amp;" "&amp;$H65&amp;" "&amp;$A65</f>
+        <f t="shared" ref="K65:T76" si="15">"zzz Infer "&amp;$A$2&amp;" Config.NoInclude/Client.xml "&amp;$G65&amp;" "&amp;K$2&amp;" "&amp;$H65&amp;" "&amp;$A65</f>
         <v>zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0.xml Config.NoInclude/Engines/SCGD-2-2-1.xml 4916</v>
       </c>
       <c r="L65" t="str">
@@ -4643,8 +4687,20 @@
         <f t="shared" si="15"/>
         <v>zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/SCGD-2-2-1.xml 4916</v>
       </c>
-    </row>
-    <row r="66" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+      <c r="R65" t="str">
+        <f t="shared" si="15"/>
+        <v>zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0a-bsc1.xml Config.NoInclude/Engines/SCGD-2-2-1.xml 4916</v>
+      </c>
+      <c r="S65" t="str">
+        <f t="shared" si="15"/>
+        <v>zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0b-bsc1.xml Config.NoInclude/Engines/SCGD-2-2-1.xml 4916</v>
+      </c>
+      <c r="T65" t="str">
+        <f t="shared" si="15"/>
+        <v>zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0c-bsc1.xml Config.NoInclude/Engines/SCGD-2-2-1.xml 4916</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B66" t="s">
         <v>0</v>
       </c>
@@ -4706,7 +4762,7 @@
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/SCGD-2-2-1.xml </v>
       </c>
     </row>
-    <row r="67" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B67" t="s">
         <v>0</v>
       </c>
@@ -4768,7 +4824,7 @@
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/SCGD-2-2-1.xml </v>
       </c>
     </row>
-    <row r="68" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B68" t="s">
         <v>0</v>
       </c>
@@ -4830,7 +4886,7 @@
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/SCGD-2-2-1.xml </v>
       </c>
     </row>
-    <row r="69" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
         <v>0</v>
       </c>
@@ -4892,7 +4948,7 @@
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/SCGD-2-2-1.xml </v>
       </c>
     </row>
-    <row r="70" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
         <v>0</v>
       </c>
@@ -4954,7 +5010,7 @@
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/SCGD-2-2-1.xml </v>
       </c>
     </row>
-    <row r="71" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B71" t="s">
         <v>0</v>
       </c>
@@ -5016,7 +5072,7 @@
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/SCGD-2-2-1.xml </v>
       </c>
     </row>
-    <row r="72" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B72" t="s">
         <v>0</v>
       </c>
@@ -5078,7 +5134,7 @@
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/SCGD-2-2-1.xml </v>
       </c>
     </row>
-    <row r="73" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B73" t="s">
         <v>0</v>
       </c>
@@ -5140,7 +5196,7 @@
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/200-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/SCGD-2-2-1.xml </v>
       </c>
     </row>
-    <row r="74" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
         <v>0</v>
       </c>
@@ -5202,7 +5258,7 @@
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/050-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/SCGD-2-2-1.xml </v>
       </c>
     </row>
-    <row r="75" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B75" t="s">
         <v>0</v>
       </c>
@@ -5264,7 +5320,7 @@
         <v xml:space="preserve">zzz Infer 22 Config.NoInclude/Client.xml Config.NoInclude/DataShapes/100-1.xml Config.NoInclude/DataSets/i0d.xml Config.NoInclude/Engines/SCGD-2-2-1.xml </v>
       </c>
     </row>
-    <row r="76" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
       <c r="B76" t="s">
         <v>0</v>
       </c>
@@ -5328,6 +5384,11 @@
     </row>
   </sheetData>
   <autoFilter ref="A4:Q76">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="SCGD"/>
+      </filters>
+    </filterColumn>
     <filterColumn colId="3">
       <filters>
         <filter val="06000"/>
@@ -5340,5 +5401,6 @@
     </filterColumn>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>